<commit_message>
added aggregated count of services for categories, duration in program
</commit_message>
<xml_diff>
--- a/templates/excel_template/individual_service_layering_template.xlsx
+++ b/templates/excel_template/individual_service_layering_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20040" tabRatio="500"/>
+    <workbookView xWindow="36140" yWindow="4400" windowWidth="29480" windowHeight="14680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Services_Received" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>ANC/PMTCT</t>
   </si>
@@ -279,6 +279,24 @@
   </si>
   <si>
     <t>Date Exited</t>
+  </si>
+  <si>
+    <t>duration_in_dreams_program</t>
+  </si>
+  <si>
+    <t>Behavioral</t>
+  </si>
+  <si>
+    <t>Bio-Medical</t>
+  </si>
+  <si>
+    <t>Post-GBV Care</t>
+  </si>
+  <si>
+    <t>Social Protection</t>
+  </si>
+  <si>
+    <t>Other Interventions</t>
   </si>
 </sst>
 </file>
@@ -602,7 +620,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CF1"/>
+  <dimension ref="A1:CL1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -611,7 +629,7 @@
     <col min="9" max="9" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:90" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -859,9 +877,27 @@
         <v>80</v>
       </c>
       <c r="CE1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CK1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added months to duration in program column
</commit_message>
<xml_diff>
--- a/templates/excel_template/individual_service_layering_template.xlsx
+++ b/templates/excel_template/individual_service_layering_template.xlsx
@@ -281,9 +281,6 @@
     <t>Date Exited</t>
   </si>
   <si>
-    <t>duration_in_dreams_program</t>
-  </si>
-  <si>
     <t>Behavioral</t>
   </si>
   <si>
@@ -297,6 +294,9 @@
   </si>
   <si>
     <t>Other Interventions</t>
+  </si>
+  <si>
+    <t>duration_in_dreams_program_in_months</t>
   </si>
 </sst>
 </file>
@@ -877,22 +877,22 @@
         <v>80</v>
       </c>
       <c r="CE1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CF1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="CJ1" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="CK1" s="1" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
F030. Split PrEP Given and PrEP Education in Services received export
</commit_message>
<xml_diff>
--- a/templates/excel_template/individual_service_layering_template.xlsx
+++ b/templates/excel_template/individual_service_layering_template.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonyojwang/myprojects/pythonProjects/dreams-database/templates/excel_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amos.laboso/Developer/dreams-database/templates/excel_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329EA996-70CA-1446-BCDB-1EBEB3887285}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36140" yWindow="4400" windowWidth="29480" windowHeight="14680" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="680" windowWidth="27320" windowHeight="14680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Services_Received" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>ANC/PMTCT</t>
   </si>
@@ -107,9 +108,6 @@
     <t>Pregnancy Test</t>
   </si>
   <si>
-    <t>PrEP</t>
-  </si>
-  <si>
     <t>RESPECT-K</t>
   </si>
   <si>
@@ -297,12 +295,18 @@
   </si>
   <si>
     <t>duration_in_dreams_program_in_months</t>
+  </si>
+  <si>
+    <t>PrEP Given</t>
+  </si>
+  <si>
+    <t>PrEP Education</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -352,6 +356,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -619,61 +626,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CL1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:CM1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AS12" sqref="AS12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="9" max="9" width="21.83203125" customWidth="1"/>
+    <col min="43" max="43" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:90" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:91" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>16</v>
@@ -682,52 +692,52 @@
         <v>19</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="W1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>18</v>
@@ -739,166 +749,169 @@
         <v>3</v>
       </c>
       <c r="AK1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AT1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AR1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AV1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AT1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AY1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AW1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="BA1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AY1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="BD1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BB1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="BT1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BI1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BW1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BT1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BX1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="BY1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="CC1" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="CB1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="CC1" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="CD1" s="1" t="s">
         <v>80</v>
       </c>
       <c r="CE1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="CG1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CK1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="CJ1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="CK1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="CM1" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="CL1" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>